<commit_message>
Updating state policy data
new states issued closure orders
</commit_message>
<xml_diff>
--- a/data/covid_closures_by_state.xlsx
+++ b/data/covid_closures_by_state.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethpancotti/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethpancotti/Documents/GitHub/GoogleTrendsUINowcast/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5174DB5-D4C6-4D46-919D-4D5B179710A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52540976-E2F0-564D-A467-11114996000C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20440" yWindow="460" windowWidth="16620" windowHeight="14940" xr2:uid="{2E3C4A39-8A20-E24A-9F68-913CA19D2F72}"/>
+    <workbookView xWindow="1440" yWindow="820" windowWidth="16620" windowHeight="14940" xr2:uid="{2E3C4A39-8A20-E24A-9F68-913CA19D2F72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="168">
   <si>
     <t>state</t>
   </si>
@@ -522,9 +522,6 @@
   </si>
   <si>
     <t>3/17/20 was first wave of partial closures (clubs, gyms, spas, theaters)</t>
-  </si>
-  <si>
-    <t>no statewide order, but 3/30/20 stay at home order issues for SE FL</t>
   </si>
   <si>
     <t>partial closure didn't limit restaurants to take out only</t>
@@ -909,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD148692-B53F-0146-860F-EA659C5658BF}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1137,8 +1134,8 @@
       <c r="E11" s="1">
         <v>43910</v>
       </c>
-      <c r="G11" t="s">
-        <v>163</v>
+      <c r="F11" s="1">
+        <v>43924</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1157,6 +1154,9 @@
       <c r="E12" s="1">
         <v>43914</v>
       </c>
+      <c r="F12" s="1">
+        <v>43924</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1275,7 +1275,7 @@
         <v>43920</v>
       </c>
       <c r="G18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1435,7 +1435,7 @@
         <v>43914</v>
       </c>
       <c r="G26" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1569,7 +1569,7 @@
         <v>43913</v>
       </c>
       <c r="G33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1742,6 +1742,9 @@
       <c r="E42" s="1">
         <v>43907</v>
       </c>
+      <c r="F42" s="1">
+        <v>43921</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -1760,7 +1763,7 @@
         <v>43913</v>
       </c>
       <c r="G43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -1799,6 +1802,9 @@
       <c r="E45" s="1">
         <v>43910</v>
       </c>
+      <c r="F45" s="1">
+        <v>43923</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -1820,7 +1826,7 @@
         <v>43917</v>
       </c>
       <c r="G46" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
new graphs based on paul's email
</commit_message>
<xml_diff>
--- a/data/covid_closures_by_state.xlsx
+++ b/data/covid_closures_by_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethpancotti/Documents/GitHub/GoogleTrendsUINowcast/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52540976-E2F0-564D-A467-11114996000C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE46288F-CD33-2E4A-837A-7DD6A14A3B0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="820" windowWidth="16620" windowHeight="14940" xr2:uid="{2E3C4A39-8A20-E24A-9F68-913CA19D2F72}"/>
   </bookViews>
@@ -906,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD148692-B53F-0146-860F-EA659C5658BF}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1191,6 +1191,9 @@
       <c r="D14" s="1">
         <v>43913</v>
       </c>
+      <c r="E14" s="1">
+        <v>43915</v>
+      </c>
       <c r="F14" s="1">
         <v>43915</v>
       </c>
@@ -1505,6 +1508,9 @@
       <c r="D30" s="1">
         <v>43906</v>
       </c>
+      <c r="E30" s="1">
+        <v>43908</v>
+      </c>
       <c r="F30" s="1">
         <v>43908</v>
       </c>
@@ -1661,6 +1667,9 @@
       </c>
       <c r="D38" s="1">
         <v>43907</v>
+      </c>
+      <c r="E38" s="1">
+        <v>43915</v>
       </c>
       <c r="F38" s="1">
         <v>43915</v>

</xml_diff>